<commit_message>
Added last participant's responses
</commit_message>
<xml_diff>
--- a/BASL_exp2.2_participants.xlsx
+++ b/BASL_exp2.2_participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a66c9eafe7ca5b97/Documents/GitHub/affixproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="8_{887243C0-272B-402E-8C9C-DBC0A0327768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98DD75D6-99AC-432D-9129-C14D7DA0580E}"/>
+  <xr:revisionPtr revIDLastSave="819" documentId="8_{887243C0-272B-402E-8C9C-DBC0A0327768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB94B690-D367-4100-AEC0-709A034FBE02}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6860" yWindow="350" windowWidth="12790" windowHeight="6550" activeTab="1" xr2:uid="{308C4EC2-7A69-4E87-98B0-7A0BAA14F23A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{308C4EC2-7A69-4E87-98B0-7A0BAA14F23A}"/>
   </bookViews>
   <sheets>
     <sheet name="Prolific" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="286">
   <si>
     <t>ID</t>
   </si>
@@ -892,6 +892,9 @@
   </si>
   <si>
     <t>669cc52163cce3554e97d184</t>
+  </si>
+  <si>
+    <t>{"ProfSpeakL1":"6","ProfUnderstandL1":"6","ProfReadL1":"6","AttentionL1":"2","ProfWriteL1":"6"}; {"AttSelfL1":"6","AttCultureL1":"6","AttNativeLevelL1":"6","AttMothertongueL1":"6"}</t>
   </si>
 </sst>
 </file>
@@ -929,7 +932,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,12 +942,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1076,12 +1073,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1558,9 +1553,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D238B1F3-D3D4-4176-AFE6-65BC297A2199}">
   <dimension ref="A1:AH191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1723,7 +1718,7 @@
       </c>
       <c r="H3" s="7" t="str">
         <f>"Approved: " &amp; COUNTIF(N:N,"yes")</f>
-        <v>Approved: 33</v>
+        <v>Approved: 34</v>
       </c>
       <c r="J3" s="6">
         <v>2</v>
@@ -1876,7 +1871,7 @@
       </c>
       <c r="H6" s="7" t="str">
         <f>"TOTAL APPROVED: " &amp; COUNTIF(F:F,"YES")+COUNTIF(N:N,"YES")+COUNTIF(V:V,"YES")</f>
-        <v>TOTAL APPROVED: 99</v>
+        <v>TOTAL APPROVED: 100</v>
       </c>
       <c r="J6" s="6">
         <v>5</v>
@@ -2149,7 +2144,7 @@
       <c r="V11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="X11" s="21"/>
+      <c r="X11" s="20"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B12" s="6">
@@ -2473,12 +2468,6 @@
       <c r="F19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="5">
-        <v>15</v>
-      </c>
-      <c r="I19" s="5">
-        <v>450</v>
-      </c>
       <c r="J19" s="6">
         <v>19</v>
       </c>
@@ -2527,21 +2516,20 @@
       <c r="F20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="5">
-        <v>9</v>
-      </c>
-      <c r="I20" s="5">
-        <f>I19*H20/H19</f>
-        <v>270</v>
-      </c>
       <c r="J20" s="6">
         <v>20</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="L20" s="20" t="s">
-        <v>63</v>
+      <c r="L20" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="R20" s="6">
         <v>19</v>
@@ -2576,10 +2564,6 @@
       <c r="F21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="5">
-        <f>I20*0.8</f>
-        <v>216</v>
-      </c>
       <c r="J21" s="6">
         <v>24</v>
       </c>
@@ -2622,10 +2606,6 @@
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="5">
-        <f>I20-I21</f>
-        <v>54</v>
-      </c>
       <c r="J22" s="6">
         <v>25</v>
       </c>
@@ -2770,6 +2750,7 @@
       <c r="F25" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="G25"/>
       <c r="J25" s="6">
         <v>28</v>
       </c>
@@ -3555,7 +3536,7 @@
       <c r="X53" s="10"/>
     </row>
     <row r="54" spans="5:24" x14ac:dyDescent="0.35">
-      <c r="X54" s="21"/>
+      <c r="X54" s="20"/>
     </row>
     <row r="55" spans="5:24" x14ac:dyDescent="0.35">
       <c r="X55" s="10"/>
@@ -3588,7 +3569,7 @@
       <c r="X64" s="10"/>
     </row>
     <row r="65" spans="24:24" x14ac:dyDescent="0.35">
-      <c r="X65" s="21"/>
+      <c r="X65" s="20"/>
     </row>
     <row r="66" spans="24:24" x14ac:dyDescent="0.35">
       <c r="X66" s="10"/>
@@ -3683,10 +3664,10 @@
       <c r="X95" s="10"/>
     </row>
     <row r="96" spans="5:24" x14ac:dyDescent="0.35">
-      <c r="X96" s="21"/>
+      <c r="X96" s="20"/>
     </row>
     <row r="97" spans="24:24" x14ac:dyDescent="0.35">
-      <c r="X97" s="21"/>
+      <c r="X97" s="20"/>
     </row>
     <row r="98" spans="24:24" x14ac:dyDescent="0.35">
       <c r="X98" s="10"/>
@@ -3716,7 +3697,7 @@
       <c r="X106" s="10"/>
     </row>
     <row r="107" spans="24:24" x14ac:dyDescent="0.35">
-      <c r="X107" s="21"/>
+      <c r="X107" s="20"/>
     </row>
     <row r="108" spans="24:24" x14ac:dyDescent="0.35">
       <c r="X108" s="10"/>
@@ -3761,7 +3742,7 @@
       <c r="X121" s="10"/>
     </row>
     <row r="122" spans="24:24" x14ac:dyDescent="0.35">
-      <c r="X122" s="21"/>
+      <c r="X122" s="20"/>
     </row>
     <row r="123" spans="24:24" x14ac:dyDescent="0.35">
       <c r="X123" s="10"/>
@@ -3800,7 +3781,7 @@
       <c r="X134" s="10"/>
     </row>
     <row r="135" spans="24:24" x14ac:dyDescent="0.35">
-      <c r="X135" s="21"/>
+      <c r="X135" s="20"/>
     </row>
     <row r="136" spans="24:24" x14ac:dyDescent="0.35">
       <c r="X136" s="10"/>
@@ -3953,7 +3934,7 @@
       <c r="X185" s="10"/>
     </row>
     <row r="186" spans="24:24" x14ac:dyDescent="0.35">
-      <c r="X186" s="21"/>
+      <c r="X186" s="20"/>
     </row>
     <row r="187" spans="24:24" x14ac:dyDescent="0.35">
       <c r="X187" s="10"/>
@@ -4079,7 +4060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D959760D-4423-43A3-94B0-AD1A8EA82D78}">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>